<commit_message>
dataChanged.emit(index,index) implemented in model
</commit_message>
<xml_diff>
--- a/content_engineer_studio/ContentEngineerStudio/tests/widgets/test.xlsx
+++ b/content_engineer_studio/ContentEngineerStudio/tests/widgets/test.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24931"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Me\Dropbox\Python\content_engineer_studio\ContentEngineerStudio\tests\widgets\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE0B0319-E799-451E-B7E1-EBE251FCC7BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="-30828" yWindow="-108" windowWidth="30936" windowHeight="17496" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="978" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="979" uniqueCount="44">
   <si>
     <t>Kanal</t>
   </si>
@@ -76,10 +82,6 @@
     <t>https://www.cleverbot.com/conv/202202241133/AYAXQ45O6L_Hey-can-I-tell-you-my-super-secret-phone-number-It-is-078-554-22-64</t>
   </si>
   <si>
-    <t xml:space="preserve">ja
-</t>
-  </si>
-  <si>
     <t>Ja</t>
   </si>
   <si>
@@ -95,9 +97,6 @@
   </si>
   <si>
     <t>https://www.cleverbot.com/conv/202202071608/WXBLHBYZ88_Hello-there</t>
-  </si>
-  <si>
-    <t>nein</t>
   </si>
   <si>
     <t xml:space="preserve">Aenean tincidunt leo arcu, non facilisis felis tempus non. Proin ante augue, porttitor nec molestie ut, gravida sit amet nulla. Pellentesque felis purus, </t>
@@ -157,13 +156,22 @@
 massa rutrum sem, vitae fringilla arcu nisl in odio.
 </t>
   </si>
+  <si>
+    <t>Analysis populates correctly</t>
+  </si>
+  <si>
+    <t>Test Editable</t>
+  </si>
+  <si>
+    <t>switching is working</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="mmss.f"/>
+    <numFmt numFmtId="164" formatCode="mmss\.\f"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -202,12 +210,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFf8cbad"/>
+        <fgColor rgb="FFF8CBAD"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFffff00"/>
+        <fgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -221,16 +229,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </left>
       <right style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </right>
       <top style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </bottom>
       <diagonal/>
     </border>
@@ -246,52 +254,51 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="13">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -302,10 +309,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -343,71 +350,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -435,7 +442,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -458,11 +465,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -471,13 +478,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -487,7 +494,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -496,7 +503,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -505,7 +512,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -513,10 +520,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -581,31 +588,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:L294"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" style="11" width="12.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="12" width="12.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="11" width="19.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="12" width="17.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="11" width="12.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="12" width="13.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="11" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="12" width="16.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="12" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="12" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="12" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="12" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="12.33203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.6640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.88671875" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.6640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.5546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="12" width="14.109375" style="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="47.25" customFormat="1" s="1">
+    <row r="1" spans="1:12" s="1" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -633,11 +639,13 @@
       <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2"/>
+      <c r="J1" s="2" t="s">
+        <v>42</v>
+      </c>
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="2" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
@@ -665,11 +673,13 @@
       <c r="I2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="J2" s="3"/>
+      <c r="J2" s="4" t="s">
+        <v>13</v>
+      </c>
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="116.25" customFormat="1" s="1">
+    <row r="3" spans="1:12" s="1" customFormat="1" ht="116.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>16</v>
       </c>
@@ -685,17 +695,19 @@
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
       <c r="G3" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="H3" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="H3" s="4" t="s">
-        <v>21</v>
-      </c>
       <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
+      <c r="J3" s="4" t="s">
+        <v>43</v>
+      </c>
       <c r="K3" s="4"/>
       <c r="L3" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="157.5" customFormat="1" s="1">
+    <row r="4" spans="1:12" s="1" customFormat="1" ht="157.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>16</v>
       </c>
@@ -706,22 +718,20 @@
         <v>18</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="4"/>
+      <c r="H4" s="4" t="s">
         <v>23</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>24</v>
       </c>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
       <c r="L4" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="157.5" customFormat="1" s="1">
+    <row r="5" spans="1:12" s="1" customFormat="1" ht="157.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>16</v>
       </c>
@@ -732,22 +742,22 @@
         <v>18</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
-      <c r="G5" s="4" t="s">
-        <v>26</v>
+      <c r="G5" s="4">
+        <v>3</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
       <c r="L5" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="75">
+    <row r="6" spans="1:12" ht="75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>16</v>
       </c>
@@ -758,22 +768,22 @@
         <v>18</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="6"/>
       <c r="G6" s="7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="I6" s="6"/>
       <c r="J6" s="6"/>
       <c r="K6" s="6"/>
       <c r="L6" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="240.75">
+    <row r="7" spans="1:12" ht="240.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>16</v>
       </c>
@@ -784,22 +794,22 @@
         <v>18</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E7" s="4"/>
       <c r="F7" s="6"/>
       <c r="G7" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="I7" s="6"/>
       <c r="J7" s="6"/>
       <c r="K7" s="6"/>
       <c r="L7" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="240.75">
+    <row r="8" spans="1:12" ht="240.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>16</v>
       </c>
@@ -810,26 +820,26 @@
         <v>18</v>
       </c>
       <c r="D8" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="E8" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>35</v>
-      </c>
       <c r="G8" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I8" s="6"/>
       <c r="J8" s="6"/>
       <c r="K8" s="6"/>
       <c r="L8" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="217.5">
+    <row r="9" spans="1:12" ht="217.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>16</v>
       </c>
@@ -840,26 +850,26 @@
         <v>18</v>
       </c>
       <c r="D9" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G9" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="E9" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F9" s="4" t="s">
+      <c r="H9" s="4" t="s">
         <v>37</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>39</v>
       </c>
       <c r="I9" s="6"/>
       <c r="J9" s="6"/>
       <c r="K9" s="6"/>
       <c r="L9" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="144">
+    <row r="10" spans="1:12" ht="144" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>16</v>
       </c>
@@ -870,7 +880,7 @@
         <v>18</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E10" s="4"/>
       <c r="F10" s="6"/>
@@ -881,7 +891,7 @@
       <c r="K10" s="6"/>
       <c r="L10" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
+    <row r="11" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>16</v>
       </c>
@@ -892,7 +902,7 @@
         <v>18</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E11" s="4"/>
       <c r="F11" s="6"/>
@@ -903,7 +913,7 @@
       <c r="K11" s="6"/>
       <c r="L11" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
+    <row r="12" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>16</v>
       </c>
@@ -914,7 +924,7 @@
         <v>18</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E12" s="4"/>
       <c r="F12" s="6"/>
@@ -925,7 +935,7 @@
       <c r="K12" s="6"/>
       <c r="L12" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
+    <row r="13" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>16</v>
       </c>
@@ -936,7 +946,7 @@
         <v>18</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E13" s="4"/>
       <c r="F13" s="6"/>
@@ -947,7 +957,7 @@
       <c r="K13" s="6"/>
       <c r="L13" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
+    <row r="14" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>16</v>
       </c>
@@ -958,7 +968,7 @@
         <v>18</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E14" s="4"/>
       <c r="F14" s="6"/>
@@ -969,7 +979,7 @@
       <c r="K14" s="6"/>
       <c r="L14" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
+    <row r="15" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>16</v>
       </c>
@@ -980,7 +990,7 @@
         <v>18</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E15" s="4"/>
       <c r="F15" s="6"/>
@@ -991,7 +1001,7 @@
       <c r="K15" s="6"/>
       <c r="L15" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
+    <row r="16" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>16</v>
       </c>
@@ -1002,7 +1012,7 @@
         <v>18</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E16" s="4"/>
       <c r="F16" s="6"/>
@@ -1013,7 +1023,7 @@
       <c r="K16" s="6"/>
       <c r="L16" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
+    <row r="17" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>16</v>
       </c>
@@ -1024,7 +1034,7 @@
         <v>18</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E17" s="4"/>
       <c r="F17" s="6"/>
@@ -1035,7 +1045,7 @@
       <c r="K17" s="6"/>
       <c r="L17" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
+    <row r="18" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>16</v>
       </c>
@@ -1046,7 +1056,7 @@
         <v>18</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E18" s="8"/>
       <c r="F18" s="9"/>
@@ -1057,7 +1067,7 @@
       <c r="K18" s="10"/>
       <c r="L18" s="10"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
+    <row r="19" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>16</v>
       </c>
@@ -1068,7 +1078,7 @@
         <v>18</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E19" s="8"/>
       <c r="F19" s="9"/>
@@ -1079,7 +1089,7 @@
       <c r="K19" s="10"/>
       <c r="L19" s="10"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
+    <row r="20" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>16</v>
       </c>
@@ -1090,7 +1100,7 @@
         <v>18</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E20" s="8"/>
       <c r="F20" s="9"/>
@@ -1101,7 +1111,7 @@
       <c r="K20" s="10"/>
       <c r="L20" s="10"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
+    <row r="21" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>16</v>
       </c>
@@ -1112,7 +1122,7 @@
         <v>18</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E21" s="8"/>
       <c r="F21" s="9"/>
@@ -1123,7 +1133,7 @@
       <c r="K21" s="10"/>
       <c r="L21" s="10"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
+    <row r="22" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
         <v>16</v>
       </c>
@@ -1134,7 +1144,7 @@
         <v>18</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E22" s="8"/>
       <c r="F22" s="9"/>
@@ -1145,7 +1155,7 @@
       <c r="K22" s="10"/>
       <c r="L22" s="10"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
+    <row r="23" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
         <v>16</v>
       </c>
@@ -1156,7 +1166,7 @@
         <v>18</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E23" s="8"/>
       <c r="F23" s="9"/>
@@ -1167,7 +1177,7 @@
       <c r="K23" s="10"/>
       <c r="L23" s="10"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
+    <row r="24" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
         <v>16</v>
       </c>
@@ -1178,7 +1188,7 @@
         <v>18</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E24" s="8"/>
       <c r="F24" s="9"/>
@@ -1189,7 +1199,7 @@
       <c r="K24" s="10"/>
       <c r="L24" s="10"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
+    <row r="25" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
         <v>16</v>
       </c>
@@ -1200,7 +1210,7 @@
         <v>18</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E25" s="8"/>
       <c r="F25" s="9"/>
@@ -1211,7 +1221,7 @@
       <c r="K25" s="10"/>
       <c r="L25" s="10"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="26" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
         <v>16</v>
       </c>
@@ -1222,7 +1232,7 @@
         <v>18</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
@@ -1233,7 +1243,7 @@
       <c r="K26" s="3"/>
       <c r="L26" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="27" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
         <v>16</v>
       </c>
@@ -1244,7 +1254,7 @@
         <v>18</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
@@ -1255,7 +1265,7 @@
       <c r="K27" s="3"/>
       <c r="L27" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="28" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
         <v>16</v>
       </c>
@@ -1266,7 +1276,7 @@
         <v>18</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
@@ -1277,7 +1287,7 @@
       <c r="K28" s="3"/>
       <c r="L28" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="29" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
         <v>16</v>
       </c>
@@ -1288,7 +1298,7 @@
         <v>18</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
@@ -1299,7 +1309,7 @@
       <c r="K29" s="3"/>
       <c r="L29" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="30" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
         <v>16</v>
       </c>
@@ -1310,7 +1320,7 @@
         <v>18</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
@@ -1321,7 +1331,7 @@
       <c r="K30" s="3"/>
       <c r="L30" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="31" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
         <v>16</v>
       </c>
@@ -1332,7 +1342,7 @@
         <v>18</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
@@ -1343,7 +1353,7 @@
       <c r="K31" s="3"/>
       <c r="L31" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="32" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
         <v>16</v>
       </c>
@@ -1354,7 +1364,7 @@
         <v>18</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
@@ -1365,7 +1375,7 @@
       <c r="K32" s="3"/>
       <c r="L32" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="33" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
         <v>16</v>
       </c>
@@ -1376,7 +1386,7 @@
         <v>18</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
@@ -1387,7 +1397,7 @@
       <c r="K33" s="3"/>
       <c r="L33" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="19.5">
+    <row r="34" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
         <v>16</v>
       </c>
@@ -1398,30 +1408,30 @@
         <v>18</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E34" s="4"/>
       <c r="F34" s="6"/>
       <c r="G34" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H34" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="I34" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J34" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="K34" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L34" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="19.5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
         <v>16</v>
       </c>
@@ -1432,30 +1442,30 @@
         <v>18</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E35" s="4"/>
       <c r="F35" s="6"/>
       <c r="G35" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H35" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I35" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H35" s="4" t="s">
+      <c r="J35" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="K35" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="I35" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="J35" s="4" t="s">
+      <c r="L35" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="K35" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="L35" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="19.5">
+    </row>
+    <row r="36" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
         <v>16</v>
       </c>
@@ -1466,7 +1476,7 @@
         <v>18</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E36" s="4"/>
       <c r="F36" s="6"/>
@@ -1477,7 +1487,7 @@
       <c r="K36" s="6"/>
       <c r="L36" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="19.5">
+    <row r="37" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="4" t="s">
         <v>16</v>
       </c>
@@ -1488,7 +1498,7 @@
         <v>18</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E37" s="4"/>
       <c r="F37" s="6"/>
@@ -1499,7 +1509,7 @@
       <c r="K37" s="6"/>
       <c r="L37" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="19.5">
+    <row r="38" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
         <v>16</v>
       </c>
@@ -1510,7 +1520,7 @@
         <v>18</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E38" s="4"/>
       <c r="F38" s="6"/>
@@ -1521,7 +1531,7 @@
       <c r="K38" s="6"/>
       <c r="L38" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="19.5">
+    <row r="39" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="4" t="s">
         <v>16</v>
       </c>
@@ -1532,7 +1542,7 @@
         <v>18</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E39" s="4"/>
       <c r="F39" s="6"/>
@@ -1543,7 +1553,7 @@
       <c r="K39" s="6"/>
       <c r="L39" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="19.5">
+    <row r="40" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="s">
         <v>16</v>
       </c>
@@ -1554,7 +1564,7 @@
         <v>18</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E40" s="4"/>
       <c r="F40" s="6"/>
@@ -1565,7 +1575,7 @@
       <c r="K40" s="6"/>
       <c r="L40" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="19.5">
+    <row r="41" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
         <v>16</v>
       </c>
@@ -1576,7 +1586,7 @@
         <v>18</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E41" s="4"/>
       <c r="F41" s="6"/>
@@ -1587,7 +1597,7 @@
       <c r="K41" s="6"/>
       <c r="L41" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="19.5">
+    <row r="42" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="s">
         <v>16</v>
       </c>
@@ -1598,7 +1608,7 @@
         <v>18</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E42" s="4"/>
       <c r="F42" s="6"/>
@@ -1609,7 +1619,7 @@
       <c r="K42" s="6"/>
       <c r="L42" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="19.5">
+    <row r="43" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="4" t="s">
         <v>16</v>
       </c>
@@ -1620,7 +1630,7 @@
         <v>18</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E43" s="4"/>
       <c r="F43" s="6"/>
@@ -1631,7 +1641,7 @@
       <c r="K43" s="6"/>
       <c r="L43" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="19.5">
+    <row r="44" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="4" t="s">
         <v>16</v>
       </c>
@@ -1642,7 +1652,7 @@
         <v>18</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E44" s="4"/>
       <c r="F44" s="6"/>
@@ -1653,7 +1663,7 @@
       <c r="K44" s="6"/>
       <c r="L44" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="19.5">
+    <row r="45" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="4" t="s">
         <v>16</v>
       </c>
@@ -1664,7 +1674,7 @@
         <v>18</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E45" s="4"/>
       <c r="F45" s="6"/>
@@ -1675,7 +1685,7 @@
       <c r="K45" s="6"/>
       <c r="L45" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="19.5">
+    <row r="46" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="4" t="s">
         <v>16</v>
       </c>
@@ -1686,7 +1696,7 @@
         <v>18</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E46" s="4"/>
       <c r="F46" s="6"/>
@@ -1697,7 +1707,7 @@
       <c r="K46" s="6"/>
       <c r="L46" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="19.5">
+    <row r="47" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="4" t="s">
         <v>16</v>
       </c>
@@ -1708,7 +1718,7 @@
         <v>18</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E47" s="4"/>
       <c r="F47" s="6"/>
@@ -1719,7 +1729,7 @@
       <c r="K47" s="6"/>
       <c r="L47" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="19.5">
+    <row r="48" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="4" t="s">
         <v>16</v>
       </c>
@@ -1730,7 +1740,7 @@
         <v>18</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E48" s="4"/>
       <c r="F48" s="6"/>
@@ -1741,7 +1751,7 @@
       <c r="K48" s="6"/>
       <c r="L48" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="19.5">
+    <row r="49" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="4" t="s">
         <v>16</v>
       </c>
@@ -1752,7 +1762,7 @@
         <v>18</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E49" s="4"/>
       <c r="F49" s="6"/>
@@ -1763,7 +1773,7 @@
       <c r="K49" s="6"/>
       <c r="L49" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="50" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="4" t="s">
         <v>16</v>
       </c>
@@ -1774,7 +1784,7 @@
         <v>18</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E50" s="3"/>
       <c r="F50" s="3"/>
@@ -1785,7 +1795,7 @@
       <c r="K50" s="3"/>
       <c r="L50" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="19.5">
+    <row r="51" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="4" t="s">
         <v>16</v>
       </c>
@@ -1805,7 +1815,7 @@
       <c r="K51" s="10"/>
       <c r="L51" s="10"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="19.5">
+    <row r="52" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="4" t="s">
         <v>16</v>
       </c>
@@ -1825,7 +1835,7 @@
       <c r="K52" s="10"/>
       <c r="L52" s="10"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="19.5">
+    <row r="53" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="4" t="s">
         <v>16</v>
       </c>
@@ -1845,7 +1855,7 @@
       <c r="K53" s="10"/>
       <c r="L53" s="10"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="19.5">
+    <row r="54" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="4" t="s">
         <v>16</v>
       </c>
@@ -1865,7 +1875,7 @@
       <c r="K54" s="10"/>
       <c r="L54" s="10"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="19.5">
+    <row r="55" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="4" t="s">
         <v>16</v>
       </c>
@@ -1885,7 +1895,7 @@
       <c r="K55" s="10"/>
       <c r="L55" s="10"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="19.5">
+    <row r="56" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="4" t="s">
         <v>16</v>
       </c>
@@ -1905,7 +1915,7 @@
       <c r="K56" s="10"/>
       <c r="L56" s="10"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="19.5">
+    <row r="57" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="4" t="s">
         <v>16</v>
       </c>
@@ -1925,7 +1935,7 @@
       <c r="K57" s="10"/>
       <c r="L57" s="10"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="19.5">
+    <row r="58" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="4" t="s">
         <v>16</v>
       </c>
@@ -1945,7 +1955,7 @@
       <c r="K58" s="10"/>
       <c r="L58" s="10"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="19.5">
+    <row r="59" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="4" t="s">
         <v>16</v>
       </c>
@@ -1965,7 +1975,7 @@
       <c r="K59" s="10"/>
       <c r="L59" s="10"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="19.5">
+    <row r="60" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="4" t="s">
         <v>16</v>
       </c>
@@ -1985,7 +1995,7 @@
       <c r="K60" s="10"/>
       <c r="L60" s="10"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="19.5">
+    <row r="61" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="4" t="s">
         <v>16</v>
       </c>
@@ -2005,7 +2015,7 @@
       <c r="K61" s="10"/>
       <c r="L61" s="10"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="19.5">
+    <row r="62" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="4" t="s">
         <v>16</v>
       </c>
@@ -2025,7 +2035,7 @@
       <c r="K62" s="10"/>
       <c r="L62" s="10"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="19.5">
+    <row r="63" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="4" t="s">
         <v>16</v>
       </c>
@@ -2045,7 +2055,7 @@
       <c r="K63" s="10"/>
       <c r="L63" s="10"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="19.5">
+    <row r="64" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="4" t="s">
         <v>16</v>
       </c>
@@ -2065,7 +2075,7 @@
       <c r="K64" s="10"/>
       <c r="L64" s="10"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="19.5">
+    <row r="65" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="4" t="s">
         <v>16</v>
       </c>
@@ -2085,7 +2095,7 @@
       <c r="K65" s="10"/>
       <c r="L65" s="10"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="66" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="4" t="s">
         <v>16</v>
       </c>
@@ -2105,7 +2115,7 @@
       <c r="K66" s="3"/>
       <c r="L66" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="67" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="4" t="s">
         <v>16</v>
       </c>
@@ -2125,7 +2135,7 @@
       <c r="K67" s="3"/>
       <c r="L67" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="68" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="4" t="s">
         <v>16</v>
       </c>
@@ -2145,7 +2155,7 @@
       <c r="K68" s="3"/>
       <c r="L68" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="69" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="4" t="s">
         <v>16</v>
       </c>
@@ -2165,7 +2175,7 @@
       <c r="K69" s="3"/>
       <c r="L69" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="70" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="4" t="s">
         <v>16</v>
       </c>
@@ -2185,7 +2195,7 @@
       <c r="K70" s="3"/>
       <c r="L70" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="71" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="4" t="s">
         <v>16</v>
       </c>
@@ -2205,7 +2215,7 @@
       <c r="K71" s="3"/>
       <c r="L71" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="72" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="4" t="s">
         <v>16</v>
       </c>
@@ -2225,7 +2235,7 @@
       <c r="K72" s="3"/>
       <c r="L72" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="73" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="4" t="s">
         <v>16</v>
       </c>
@@ -2245,7 +2255,7 @@
       <c r="K73" s="3"/>
       <c r="L73" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="74" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="4" t="s">
         <v>16</v>
       </c>
@@ -2265,7 +2275,7 @@
       <c r="K74" s="3"/>
       <c r="L74" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="75" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="4" t="s">
         <v>16</v>
       </c>
@@ -2285,7 +2295,7 @@
       <c r="K75" s="3"/>
       <c r="L75" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="76" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="4" t="s">
         <v>16</v>
       </c>
@@ -2305,7 +2315,7 @@
       <c r="K76" s="3"/>
       <c r="L76" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="77" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="4" t="s">
         <v>16</v>
       </c>
@@ -2325,7 +2335,7 @@
       <c r="K77" s="3"/>
       <c r="L77" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="78" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="4" t="s">
         <v>16</v>
       </c>
@@ -2345,7 +2355,7 @@
       <c r="K78" s="3"/>
       <c r="L78" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="79" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="4" t="s">
         <v>16</v>
       </c>
@@ -2365,7 +2375,7 @@
       <c r="K79" s="3"/>
       <c r="L79" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="80" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="4" t="s">
         <v>16</v>
       </c>
@@ -2385,7 +2395,7 @@
       <c r="K80" s="3"/>
       <c r="L80" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="81" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="4" t="s">
         <v>16</v>
       </c>
@@ -2405,7 +2415,7 @@
       <c r="K81" s="3"/>
       <c r="L81" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="82" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="82" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" s="4" t="s">
         <v>16</v>
       </c>
@@ -2425,7 +2435,7 @@
       <c r="K82" s="3"/>
       <c r="L82" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="83" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="83" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" s="4" t="s">
         <v>16</v>
       </c>
@@ -2445,7 +2455,7 @@
       <c r="K83" s="3"/>
       <c r="L83" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="84" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="84" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" s="4" t="s">
         <v>16</v>
       </c>
@@ -2465,7 +2475,7 @@
       <c r="K84" s="3"/>
       <c r="L84" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="85" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="85" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" s="4" t="s">
         <v>16</v>
       </c>
@@ -2485,7 +2495,7 @@
       <c r="K85" s="3"/>
       <c r="L85" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="86" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" s="4" t="s">
         <v>16</v>
       </c>
@@ -2505,7 +2515,7 @@
       <c r="K86" s="3"/>
       <c r="L86" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="87" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" s="4" t="s">
         <v>16</v>
       </c>
@@ -2525,7 +2535,7 @@
       <c r="K87" s="3"/>
       <c r="L87" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="88" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="88" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" s="4" t="s">
         <v>16</v>
       </c>
@@ -2545,7 +2555,7 @@
       <c r="K88" s="3"/>
       <c r="L88" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="89" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="89" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" s="4" t="s">
         <v>16</v>
       </c>
@@ -2565,7 +2575,7 @@
       <c r="K89" s="3"/>
       <c r="L89" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="90" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="90" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" s="4" t="s">
         <v>16</v>
       </c>
@@ -2585,7 +2595,7 @@
       <c r="K90" s="3"/>
       <c r="L90" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="91" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="91" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" s="4" t="s">
         <v>16</v>
       </c>
@@ -2605,7 +2615,7 @@
       <c r="K91" s="3"/>
       <c r="L91" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="92" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="92" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92" s="4" t="s">
         <v>16</v>
       </c>
@@ -2625,7 +2635,7 @@
       <c r="K92" s="3"/>
       <c r="L92" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="93" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="93" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93" s="4" t="s">
         <v>16</v>
       </c>
@@ -2645,7 +2655,7 @@
       <c r="K93" s="3"/>
       <c r="L93" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="94" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="94" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94" s="4" t="s">
         <v>16</v>
       </c>
@@ -2665,7 +2675,7 @@
       <c r="K94" s="3"/>
       <c r="L94" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="95" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="95" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A95" s="4" t="s">
         <v>16</v>
       </c>
@@ -2685,7 +2695,7 @@
       <c r="K95" s="3"/>
       <c r="L95" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="96" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="96" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A96" s="4" t="s">
         <v>16</v>
       </c>
@@ -2705,7 +2715,7 @@
       <c r="K96" s="3"/>
       <c r="L96" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="97" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="97" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A97" s="4" t="s">
         <v>16</v>
       </c>
@@ -2725,7 +2735,7 @@
       <c r="K97" s="3"/>
       <c r="L97" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="98" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="98" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A98" s="4" t="s">
         <v>16</v>
       </c>
@@ -2745,7 +2755,7 @@
       <c r="K98" s="3"/>
       <c r="L98" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="99" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="99" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99" s="4" t="s">
         <v>16</v>
       </c>
@@ -2765,7 +2775,7 @@
       <c r="K99" s="3"/>
       <c r="L99" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="100" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="100" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100" s="4" t="s">
         <v>16</v>
       </c>
@@ -2785,7 +2795,7 @@
       <c r="K100" s="3"/>
       <c r="L100" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="101" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="101" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101" s="4" t="s">
         <v>16</v>
       </c>
@@ -2805,7 +2815,7 @@
       <c r="K101" s="3"/>
       <c r="L101" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="102" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="102" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102" s="4" t="s">
         <v>16</v>
       </c>
@@ -2825,7 +2835,7 @@
       <c r="K102" s="3"/>
       <c r="L102" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="103" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="103" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A103" s="4" t="s">
         <v>16</v>
       </c>
@@ -2845,7 +2855,7 @@
       <c r="K103" s="3"/>
       <c r="L103" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="104" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="104" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A104" s="4" t="s">
         <v>16</v>
       </c>
@@ -2865,7 +2875,7 @@
       <c r="K104" s="3"/>
       <c r="L104" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="105" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="105" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A105" s="4" t="s">
         <v>16</v>
       </c>
@@ -2885,7 +2895,7 @@
       <c r="K105" s="3"/>
       <c r="L105" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="106" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="106" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A106" s="4" t="s">
         <v>16</v>
       </c>
@@ -2905,7 +2915,7 @@
       <c r="K106" s="3"/>
       <c r="L106" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="107" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="107" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A107" s="4" t="s">
         <v>16</v>
       </c>
@@ -2925,7 +2935,7 @@
       <c r="K107" s="3"/>
       <c r="L107" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="108" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="108" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A108" s="4" t="s">
         <v>16</v>
       </c>
@@ -2945,7 +2955,7 @@
       <c r="K108" s="3"/>
       <c r="L108" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="109" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="109" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A109" s="4" t="s">
         <v>16</v>
       </c>
@@ -2965,7 +2975,7 @@
       <c r="K109" s="3"/>
       <c r="L109" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="110" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="110" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A110" s="4" t="s">
         <v>16</v>
       </c>
@@ -2985,7 +2995,7 @@
       <c r="K110" s="3"/>
       <c r="L110" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="111" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="111" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A111" s="4" t="s">
         <v>16</v>
       </c>
@@ -3005,7 +3015,7 @@
       <c r="K111" s="3"/>
       <c r="L111" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="112" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="112" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A112" s="4" t="s">
         <v>16</v>
       </c>
@@ -3025,7 +3035,7 @@
       <c r="K112" s="3"/>
       <c r="L112" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="113" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="113" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A113" s="4" t="s">
         <v>16</v>
       </c>
@@ -3045,7 +3055,7 @@
       <c r="K113" s="3"/>
       <c r="L113" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="114" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="114" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A114" s="4" t="s">
         <v>16</v>
       </c>
@@ -3065,7 +3075,7 @@
       <c r="K114" s="3"/>
       <c r="L114" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="115" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="115" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A115" s="4" t="s">
         <v>16</v>
       </c>
@@ -3085,7 +3095,7 @@
       <c r="K115" s="3"/>
       <c r="L115" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="116" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="116" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A116" s="4" t="s">
         <v>16</v>
       </c>
@@ -3105,7 +3115,7 @@
       <c r="K116" s="3"/>
       <c r="L116" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="117" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="117" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A117" s="4" t="s">
         <v>16</v>
       </c>
@@ -3125,7 +3135,7 @@
       <c r="K117" s="3"/>
       <c r="L117" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="118" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="118" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A118" s="4" t="s">
         <v>16</v>
       </c>
@@ -3145,7 +3155,7 @@
       <c r="K118" s="3"/>
       <c r="L118" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="119" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="119" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A119" s="4" t="s">
         <v>16</v>
       </c>
@@ -3165,7 +3175,7 @@
       <c r="K119" s="3"/>
       <c r="L119" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="120" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="120" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A120" s="4" t="s">
         <v>16</v>
       </c>
@@ -3185,7 +3195,7 @@
       <c r="K120" s="3"/>
       <c r="L120" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="121" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="121" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A121" s="4" t="s">
         <v>16</v>
       </c>
@@ -3205,7 +3215,7 @@
       <c r="K121" s="3"/>
       <c r="L121" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="122" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="122" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A122" s="4" t="s">
         <v>16</v>
       </c>
@@ -3225,7 +3235,7 @@
       <c r="K122" s="3"/>
       <c r="L122" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="123" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="123" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A123" s="4" t="s">
         <v>16</v>
       </c>
@@ -3245,7 +3255,7 @@
       <c r="K123" s="3"/>
       <c r="L123" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="124" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="124" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A124" s="4" t="s">
         <v>16</v>
       </c>
@@ -3265,7 +3275,7 @@
       <c r="K124" s="3"/>
       <c r="L124" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="125" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="125" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A125" s="4" t="s">
         <v>16</v>
       </c>
@@ -3285,7 +3295,7 @@
       <c r="K125" s="3"/>
       <c r="L125" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="126" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="126" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A126" s="4" t="s">
         <v>16</v>
       </c>
@@ -3305,7 +3315,7 @@
       <c r="K126" s="3"/>
       <c r="L126" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="127" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="127" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A127" s="4" t="s">
         <v>16</v>
       </c>
@@ -3325,7 +3335,7 @@
       <c r="K127" s="3"/>
       <c r="L127" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="128" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="128" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A128" s="4" t="s">
         <v>16</v>
       </c>
@@ -3345,7 +3355,7 @@
       <c r="K128" s="3"/>
       <c r="L128" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="129" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="129" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A129" s="4" t="s">
         <v>16</v>
       </c>
@@ -3365,7 +3375,7 @@
       <c r="K129" s="3"/>
       <c r="L129" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="130" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="130" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A130" s="4" t="s">
         <v>16</v>
       </c>
@@ -3385,7 +3395,7 @@
       <c r="K130" s="3"/>
       <c r="L130" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="131" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="131" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A131" s="4" t="s">
         <v>16</v>
       </c>
@@ -3405,7 +3415,7 @@
       <c r="K131" s="3"/>
       <c r="L131" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="132" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="132" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A132" s="4" t="s">
         <v>16</v>
       </c>
@@ -3425,7 +3435,7 @@
       <c r="K132" s="3"/>
       <c r="L132" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="133" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="133" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A133" s="4" t="s">
         <v>16</v>
       </c>
@@ -3445,7 +3455,7 @@
       <c r="K133" s="3"/>
       <c r="L133" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="134" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="134" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A134" s="4" t="s">
         <v>16</v>
       </c>
@@ -3465,7 +3475,7 @@
       <c r="K134" s="3"/>
       <c r="L134" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="135" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="135" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A135" s="4" t="s">
         <v>16</v>
       </c>
@@ -3485,7 +3495,7 @@
       <c r="K135" s="3"/>
       <c r="L135" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="136" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="136" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A136" s="4" t="s">
         <v>16</v>
       </c>
@@ -3505,7 +3515,7 @@
       <c r="K136" s="3"/>
       <c r="L136" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="137" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="137" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A137" s="4" t="s">
         <v>16</v>
       </c>
@@ -3525,7 +3535,7 @@
       <c r="K137" s="3"/>
       <c r="L137" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="138" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="138" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A138" s="4" t="s">
         <v>16</v>
       </c>
@@ -3545,7 +3555,7 @@
       <c r="K138" s="3"/>
       <c r="L138" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="139" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="139" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A139" s="4" t="s">
         <v>16</v>
       </c>
@@ -3565,7 +3575,7 @@
       <c r="K139" s="3"/>
       <c r="L139" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="140" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="140" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A140" s="4" t="s">
         <v>16</v>
       </c>
@@ -3585,7 +3595,7 @@
       <c r="K140" s="3"/>
       <c r="L140" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="141" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="141" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A141" s="4" t="s">
         <v>16</v>
       </c>
@@ -3605,7 +3615,7 @@
       <c r="K141" s="3"/>
       <c r="L141" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="142" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="142" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A142" s="4" t="s">
         <v>16</v>
       </c>
@@ -3625,7 +3635,7 @@
       <c r="K142" s="3"/>
       <c r="L142" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="143" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="143" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A143" s="4" t="s">
         <v>16</v>
       </c>
@@ -3645,7 +3655,7 @@
       <c r="K143" s="3"/>
       <c r="L143" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="144" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="144" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A144" s="4" t="s">
         <v>16</v>
       </c>
@@ -3665,7 +3675,7 @@
       <c r="K144" s="3"/>
       <c r="L144" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="145" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="145" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A145" s="4" t="s">
         <v>16</v>
       </c>
@@ -3685,7 +3695,7 @@
       <c r="K145" s="3"/>
       <c r="L145" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="146" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="146" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A146" s="4" t="s">
         <v>16</v>
       </c>
@@ -3705,7 +3715,7 @@
       <c r="K146" s="3"/>
       <c r="L146" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="147" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="147" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A147" s="4" t="s">
         <v>16</v>
       </c>
@@ -3725,7 +3735,7 @@
       <c r="K147" s="3"/>
       <c r="L147" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="148" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="148" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A148" s="4" t="s">
         <v>16</v>
       </c>
@@ -3745,7 +3755,7 @@
       <c r="K148" s="3"/>
       <c r="L148" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="149" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="149" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A149" s="4" t="s">
         <v>16</v>
       </c>
@@ -3765,7 +3775,7 @@
       <c r="K149" s="3"/>
       <c r="L149" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="150" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="150" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A150" s="4" t="s">
         <v>16</v>
       </c>
@@ -3785,7 +3795,7 @@
       <c r="K150" s="3"/>
       <c r="L150" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="151" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="151" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A151" s="4" t="s">
         <v>16</v>
       </c>
@@ -3805,7 +3815,7 @@
       <c r="K151" s="3"/>
       <c r="L151" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="152" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="152" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A152" s="4" t="s">
         <v>16</v>
       </c>
@@ -3825,7 +3835,7 @@
       <c r="K152" s="3"/>
       <c r="L152" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="153" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="153" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A153" s="4" t="s">
         <v>16</v>
       </c>
@@ -3845,7 +3855,7 @@
       <c r="K153" s="3"/>
       <c r="L153" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="154" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="154" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A154" s="4" t="s">
         <v>16</v>
       </c>
@@ -3865,7 +3875,7 @@
       <c r="K154" s="3"/>
       <c r="L154" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="155" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="155" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A155" s="4" t="s">
         <v>16</v>
       </c>
@@ -3885,7 +3895,7 @@
       <c r="K155" s="3"/>
       <c r="L155" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="156" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="156" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A156" s="4" t="s">
         <v>16</v>
       </c>
@@ -3905,7 +3915,7 @@
       <c r="K156" s="3"/>
       <c r="L156" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="157" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="157" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A157" s="4" t="s">
         <v>16</v>
       </c>
@@ -3925,7 +3935,7 @@
       <c r="K157" s="3"/>
       <c r="L157" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="158" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="158" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A158" s="4" t="s">
         <v>16</v>
       </c>
@@ -3945,7 +3955,7 @@
       <c r="K158" s="3"/>
       <c r="L158" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="159" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="159" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A159" s="4" t="s">
         <v>16</v>
       </c>
@@ -3965,7 +3975,7 @@
       <c r="K159" s="3"/>
       <c r="L159" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="160" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="160" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A160" s="4" t="s">
         <v>16</v>
       </c>
@@ -3985,7 +3995,7 @@
       <c r="K160" s="3"/>
       <c r="L160" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="161" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="161" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A161" s="4" t="s">
         <v>16</v>
       </c>
@@ -4005,7 +4015,7 @@
       <c r="K161" s="3"/>
       <c r="L161" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="162" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="162" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A162" s="4" t="s">
         <v>16</v>
       </c>
@@ -4025,7 +4035,7 @@
       <c r="K162" s="3"/>
       <c r="L162" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="163" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="163" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A163" s="4" t="s">
         <v>16</v>
       </c>
@@ -4045,7 +4055,7 @@
       <c r="K163" s="3"/>
       <c r="L163" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="164" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="164" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A164" s="4" t="s">
         <v>16</v>
       </c>
@@ -4065,7 +4075,7 @@
       <c r="K164" s="3"/>
       <c r="L164" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="165" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="165" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A165" s="4" t="s">
         <v>16</v>
       </c>
@@ -4085,7 +4095,7 @@
       <c r="K165" s="3"/>
       <c r="L165" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="166" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="166" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A166" s="4" t="s">
         <v>16</v>
       </c>
@@ -4105,7 +4115,7 @@
       <c r="K166" s="3"/>
       <c r="L166" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="167" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="167" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A167" s="4" t="s">
         <v>16</v>
       </c>
@@ -4125,7 +4135,7 @@
       <c r="K167" s="3"/>
       <c r="L167" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="168" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="168" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A168" s="4" t="s">
         <v>16</v>
       </c>
@@ -4145,7 +4155,7 @@
       <c r="K168" s="3"/>
       <c r="L168" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="169" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="169" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A169" s="4" t="s">
         <v>16</v>
       </c>
@@ -4165,7 +4175,7 @@
       <c r="K169" s="3"/>
       <c r="L169" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="170" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="170" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A170" s="4" t="s">
         <v>16</v>
       </c>
@@ -4185,7 +4195,7 @@
       <c r="K170" s="3"/>
       <c r="L170" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="171" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="171" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A171" s="4" t="s">
         <v>16</v>
       </c>
@@ -4205,7 +4215,7 @@
       <c r="K171" s="3"/>
       <c r="L171" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="172" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="172" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A172" s="4" t="s">
         <v>16</v>
       </c>
@@ -4225,7 +4235,7 @@
       <c r="K172" s="3"/>
       <c r="L172" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="173" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="173" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A173" s="4" t="s">
         <v>16</v>
       </c>
@@ -4245,7 +4255,7 @@
       <c r="K173" s="3"/>
       <c r="L173" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="174" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="174" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A174" s="4" t="s">
         <v>16</v>
       </c>
@@ -4265,7 +4275,7 @@
       <c r="K174" s="3"/>
       <c r="L174" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="175" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="175" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A175" s="4" t="s">
         <v>16</v>
       </c>
@@ -4285,7 +4295,7 @@
       <c r="K175" s="3"/>
       <c r="L175" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="176" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="176" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A176" s="4" t="s">
         <v>16</v>
       </c>
@@ -4305,7 +4315,7 @@
       <c r="K176" s="3"/>
       <c r="L176" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="177" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="177" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A177" s="4" t="s">
         <v>16</v>
       </c>
@@ -4325,7 +4335,7 @@
       <c r="K177" s="3"/>
       <c r="L177" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="178" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="178" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A178" s="4" t="s">
         <v>16</v>
       </c>
@@ -4345,7 +4355,7 @@
       <c r="K178" s="3"/>
       <c r="L178" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="179" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="179" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A179" s="4" t="s">
         <v>16</v>
       </c>
@@ -4365,7 +4375,7 @@
       <c r="K179" s="3"/>
       <c r="L179" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="180" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="180" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A180" s="4" t="s">
         <v>16</v>
       </c>
@@ -4385,7 +4395,7 @@
       <c r="K180" s="3"/>
       <c r="L180" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="181" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="181" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A181" s="4" t="s">
         <v>16</v>
       </c>
@@ -4405,7 +4415,7 @@
       <c r="K181" s="3"/>
       <c r="L181" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="182" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="182" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A182" s="4" t="s">
         <v>16</v>
       </c>
@@ -4425,7 +4435,7 @@
       <c r="K182" s="3"/>
       <c r="L182" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="183" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="183" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A183" s="4" t="s">
         <v>16</v>
       </c>
@@ -4445,7 +4455,7 @@
       <c r="K183" s="3"/>
       <c r="L183" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="184" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="184" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A184" s="4" t="s">
         <v>16</v>
       </c>
@@ -4465,7 +4475,7 @@
       <c r="K184" s="3"/>
       <c r="L184" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="185" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="185" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A185" s="4" t="s">
         <v>16</v>
       </c>
@@ -4485,7 +4495,7 @@
       <c r="K185" s="3"/>
       <c r="L185" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="186" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="186" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A186" s="4" t="s">
         <v>16</v>
       </c>
@@ -4505,7 +4515,7 @@
       <c r="K186" s="3"/>
       <c r="L186" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="187" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="187" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A187" s="4" t="s">
         <v>16</v>
       </c>
@@ -4525,7 +4535,7 @@
       <c r="K187" s="3"/>
       <c r="L187" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="188" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="188" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A188" s="4" t="s">
         <v>16</v>
       </c>
@@ -4545,7 +4555,7 @@
       <c r="K188" s="3"/>
       <c r="L188" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="189" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="189" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A189" s="4" t="s">
         <v>16</v>
       </c>
@@ -4565,7 +4575,7 @@
       <c r="K189" s="3"/>
       <c r="L189" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="190" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="190" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A190" s="4" t="s">
         <v>16</v>
       </c>
@@ -4585,7 +4595,7 @@
       <c r="K190" s="3"/>
       <c r="L190" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="191" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="191" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A191" s="4" t="s">
         <v>16</v>
       </c>
@@ -4605,7 +4615,7 @@
       <c r="K191" s="3"/>
       <c r="L191" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="192" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="192" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A192" s="4" t="s">
         <v>16</v>
       </c>
@@ -4625,7 +4635,7 @@
       <c r="K192" s="3"/>
       <c r="L192" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="193" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="193" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A193" s="4" t="s">
         <v>16</v>
       </c>
@@ -4645,7 +4655,7 @@
       <c r="K193" s="3"/>
       <c r="L193" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="194" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="194" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A194" s="4" t="s">
         <v>16</v>
       </c>
@@ -4665,7 +4675,7 @@
       <c r="K194" s="3"/>
       <c r="L194" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="195" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="195" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A195" s="4" t="s">
         <v>16</v>
       </c>
@@ -4685,7 +4695,7 @@
       <c r="K195" s="3"/>
       <c r="L195" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="196" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="196" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A196" s="4" t="s">
         <v>16</v>
       </c>
@@ -4705,7 +4715,7 @@
       <c r="K196" s="3"/>
       <c r="L196" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="197" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="197" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A197" s="4" t="s">
         <v>16</v>
       </c>
@@ -4725,7 +4735,7 @@
       <c r="K197" s="3"/>
       <c r="L197" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="198" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="198" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A198" s="4" t="s">
         <v>16</v>
       </c>
@@ -4745,7 +4755,7 @@
       <c r="K198" s="3"/>
       <c r="L198" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="199" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="199" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A199" s="4" t="s">
         <v>16</v>
       </c>
@@ -4765,7 +4775,7 @@
       <c r="K199" s="3"/>
       <c r="L199" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="200" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="200" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A200" s="4" t="s">
         <v>16</v>
       </c>
@@ -4785,7 +4795,7 @@
       <c r="K200" s="3"/>
       <c r="L200" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="201" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="201" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A201" s="4" t="s">
         <v>16</v>
       </c>
@@ -4805,7 +4815,7 @@
       <c r="K201" s="3"/>
       <c r="L201" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="202" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="202" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A202" s="4" t="s">
         <v>16</v>
       </c>
@@ -4825,7 +4835,7 @@
       <c r="K202" s="3"/>
       <c r="L202" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="203" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="203" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A203" s="4" t="s">
         <v>16</v>
       </c>
@@ -4845,7 +4855,7 @@
       <c r="K203" s="3"/>
       <c r="L203" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="204" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="204" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A204" s="4" t="s">
         <v>16</v>
       </c>
@@ -4865,7 +4875,7 @@
       <c r="K204" s="3"/>
       <c r="L204" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="205" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="205" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A205" s="4" t="s">
         <v>16</v>
       </c>
@@ -4885,7 +4895,7 @@
       <c r="K205" s="3"/>
       <c r="L205" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="206" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="206" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A206" s="4" t="s">
         <v>16</v>
       </c>
@@ -4905,7 +4915,7 @@
       <c r="K206" s="3"/>
       <c r="L206" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="207" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="207" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A207" s="4" t="s">
         <v>16</v>
       </c>
@@ -4925,7 +4935,7 @@
       <c r="K207" s="3"/>
       <c r="L207" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="208" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="208" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A208" s="4" t="s">
         <v>16</v>
       </c>
@@ -4945,7 +4955,7 @@
       <c r="K208" s="3"/>
       <c r="L208" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="209" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="209" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A209" s="4" t="s">
         <v>16</v>
       </c>
@@ -4965,7 +4975,7 @@
       <c r="K209" s="3"/>
       <c r="L209" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="210" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="210" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A210" s="4" t="s">
         <v>16</v>
       </c>
@@ -4985,7 +4995,7 @@
       <c r="K210" s="3"/>
       <c r="L210" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="211" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="211" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A211" s="4" t="s">
         <v>16</v>
       </c>
@@ -5005,7 +5015,7 @@
       <c r="K211" s="3"/>
       <c r="L211" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="212" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="212" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A212" s="4" t="s">
         <v>16</v>
       </c>
@@ -5025,7 +5035,7 @@
       <c r="K212" s="3"/>
       <c r="L212" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="213" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="213" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A213" s="4" t="s">
         <v>16</v>
       </c>
@@ -5045,7 +5055,7 @@
       <c r="K213" s="3"/>
       <c r="L213" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="214" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="214" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A214" s="4" t="s">
         <v>16</v>
       </c>
@@ -5065,7 +5075,7 @@
       <c r="K214" s="3"/>
       <c r="L214" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="215" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="215" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A215" s="4" t="s">
         <v>16</v>
       </c>
@@ -5085,7 +5095,7 @@
       <c r="K215" s="3"/>
       <c r="L215" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="216" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="216" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A216" s="4" t="s">
         <v>16</v>
       </c>
@@ -5105,7 +5115,7 @@
       <c r="K216" s="3"/>
       <c r="L216" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="217" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="217" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A217" s="4" t="s">
         <v>16</v>
       </c>
@@ -5125,7 +5135,7 @@
       <c r="K217" s="3"/>
       <c r="L217" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="218" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="218" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A218" s="4" t="s">
         <v>16</v>
       </c>
@@ -5145,7 +5155,7 @@
       <c r="K218" s="3"/>
       <c r="L218" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="219" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="219" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A219" s="4" t="s">
         <v>16</v>
       </c>
@@ -5165,7 +5175,7 @@
       <c r="K219" s="3"/>
       <c r="L219" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="220" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="220" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A220" s="4" t="s">
         <v>16</v>
       </c>
@@ -5185,7 +5195,7 @@
       <c r="K220" s="3"/>
       <c r="L220" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="221" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="221" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A221" s="4" t="s">
         <v>16</v>
       </c>
@@ -5205,7 +5215,7 @@
       <c r="K221" s="3"/>
       <c r="L221" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="222" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="222" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A222" s="4" t="s">
         <v>16</v>
       </c>
@@ -5225,7 +5235,7 @@
       <c r="K222" s="3"/>
       <c r="L222" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="223" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="223" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A223" s="4" t="s">
         <v>16</v>
       </c>
@@ -5245,7 +5255,7 @@
       <c r="K223" s="3"/>
       <c r="L223" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="224" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="224" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A224" s="4" t="s">
         <v>16</v>
       </c>
@@ -5265,7 +5275,7 @@
       <c r="K224" s="3"/>
       <c r="L224" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="225" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="225" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A225" s="4" t="s">
         <v>16</v>
       </c>
@@ -5285,7 +5295,7 @@
       <c r="K225" s="3"/>
       <c r="L225" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="226" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="226" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A226" s="4" t="s">
         <v>16</v>
       </c>
@@ -5305,7 +5315,7 @@
       <c r="K226" s="3"/>
       <c r="L226" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="227" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="227" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A227" s="4" t="s">
         <v>16</v>
       </c>
@@ -5325,7 +5335,7 @@
       <c r="K227" s="3"/>
       <c r="L227" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="228" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="228" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A228" s="4" t="s">
         <v>16</v>
       </c>
@@ -5345,7 +5355,7 @@
       <c r="K228" s="3"/>
       <c r="L228" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="229" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="229" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A229" s="4" t="s">
         <v>16</v>
       </c>
@@ -5365,7 +5375,7 @@
       <c r="K229" s="3"/>
       <c r="L229" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="230" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="230" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A230" s="4" t="s">
         <v>16</v>
       </c>
@@ -5385,7 +5395,7 @@
       <c r="K230" s="3"/>
       <c r="L230" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="231" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="231" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A231" s="4" t="s">
         <v>16</v>
       </c>
@@ -5405,7 +5415,7 @@
       <c r="K231" s="3"/>
       <c r="L231" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="232" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="232" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A232" s="4" t="s">
         <v>16</v>
       </c>
@@ -5425,7 +5435,7 @@
       <c r="K232" s="3"/>
       <c r="L232" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="233" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="233" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A233" s="4" t="s">
         <v>16</v>
       </c>
@@ -5445,7 +5455,7 @@
       <c r="K233" s="3"/>
       <c r="L233" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="234" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="234" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A234" s="4" t="s">
         <v>16</v>
       </c>
@@ -5465,7 +5475,7 @@
       <c r="K234" s="3"/>
       <c r="L234" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="235" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="235" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A235" s="4" t="s">
         <v>16</v>
       </c>
@@ -5485,7 +5495,7 @@
       <c r="K235" s="3"/>
       <c r="L235" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="236" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="236" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A236" s="4" t="s">
         <v>16</v>
       </c>
@@ -5505,7 +5515,7 @@
       <c r="K236" s="3"/>
       <c r="L236" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="237" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="237" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A237" s="4" t="s">
         <v>16</v>
       </c>
@@ -5525,7 +5535,7 @@
       <c r="K237" s="3"/>
       <c r="L237" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="238" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="238" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A238" s="4" t="s">
         <v>16</v>
       </c>
@@ -5545,7 +5555,7 @@
       <c r="K238" s="3"/>
       <c r="L238" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="239" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="239" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A239" s="4" t="s">
         <v>16</v>
       </c>
@@ -5565,7 +5575,7 @@
       <c r="K239" s="3"/>
       <c r="L239" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="240" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="240" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A240" s="4" t="s">
         <v>16</v>
       </c>
@@ -5585,7 +5595,7 @@
       <c r="K240" s="3"/>
       <c r="L240" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="241" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="241" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A241" s="4" t="s">
         <v>16</v>
       </c>
@@ -5605,7 +5615,7 @@
       <c r="K241" s="3"/>
       <c r="L241" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="242" customHeight="1" ht="19.5">
+    <row r="242" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A242" s="4" t="s">
         <v>16</v>
       </c>
@@ -5625,7 +5635,7 @@
       <c r="K242" s="10"/>
       <c r="L242" s="10"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="243" customHeight="1" ht="19.5">
+    <row r="243" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A243" s="4" t="s">
         <v>16</v>
       </c>
@@ -5645,7 +5655,7 @@
       <c r="K243" s="10"/>
       <c r="L243" s="10"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="244" customHeight="1" ht="19.5">
+    <row r="244" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A244" s="4" t="s">
         <v>16</v>
       </c>
@@ -5665,7 +5675,7 @@
       <c r="K244" s="10"/>
       <c r="L244" s="10"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="245" customHeight="1" ht="19.5">
+    <row r="245" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A245" s="4" t="s">
         <v>16</v>
       </c>
@@ -5685,7 +5695,7 @@
       <c r="K245" s="10"/>
       <c r="L245" s="10"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="246" customHeight="1" ht="19.5">
+    <row r="246" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A246" s="4" t="s">
         <v>16</v>
       </c>
@@ -5705,7 +5715,7 @@
       <c r="K246" s="10"/>
       <c r="L246" s="10"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="247" customHeight="1" ht="19.5">
+    <row r="247" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A247" s="4" t="s">
         <v>16</v>
       </c>
@@ -5725,7 +5735,7 @@
       <c r="K247" s="10"/>
       <c r="L247" s="10"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="248" customHeight="1" ht="19.5">
+    <row r="248" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A248" s="4" t="s">
         <v>16</v>
       </c>
@@ -5745,7 +5755,7 @@
       <c r="K248" s="10"/>
       <c r="L248" s="10"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="249" customHeight="1" ht="19.5">
+    <row r="249" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A249" s="4" t="s">
         <v>16</v>
       </c>
@@ -5757,23 +5767,23 @@
       </c>
       <c r="D249" s="6"/>
       <c r="E249" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F249" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G249" s="4"/>
       <c r="H249" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="I249" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J249" s="10"/>
       <c r="K249" s="10"/>
       <c r="L249" s="10"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="250" customHeight="1" ht="19.5">
+    <row r="250" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A250" s="4" t="s">
         <v>16</v>
       </c>
@@ -5785,23 +5795,23 @@
       </c>
       <c r="D250" s="6"/>
       <c r="E250" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F250" s="4" t="s">
         <v>23</v>
-      </c>
-      <c r="F250" s="4" t="s">
-        <v>24</v>
       </c>
       <c r="G250" s="4"/>
       <c r="H250" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I250" s="4" t="s">
         <v>23</v>
-      </c>
-      <c r="I250" s="4" t="s">
-        <v>24</v>
       </c>
       <c r="J250" s="10"/>
       <c r="K250" s="10"/>
       <c r="L250" s="10"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="251" customHeight="1" ht="19.5">
+    <row r="251" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A251" s="4" t="s">
         <v>16</v>
       </c>
@@ -5821,7 +5831,7 @@
       <c r="K251" s="10"/>
       <c r="L251" s="10"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="252" customHeight="1" ht="19.5">
+    <row r="252" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A252" s="4" t="s">
         <v>16</v>
       </c>
@@ -5841,7 +5851,7 @@
       <c r="K252" s="10"/>
       <c r="L252" s="10"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="253" customHeight="1" ht="19.5">
+    <row r="253" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A253" s="4" t="s">
         <v>16</v>
       </c>
@@ -5861,7 +5871,7 @@
       <c r="K253" s="10"/>
       <c r="L253" s="10"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="254" customHeight="1" ht="19.5">
+    <row r="254" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A254" s="4" t="s">
         <v>16</v>
       </c>
@@ -5881,7 +5891,7 @@
       <c r="K254" s="10"/>
       <c r="L254" s="10"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="255" customHeight="1" ht="19.5">
+    <row r="255" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A255" s="4" t="s">
         <v>16</v>
       </c>
@@ -5901,7 +5911,7 @@
       <c r="K255" s="10"/>
       <c r="L255" s="10"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="256" customHeight="1" ht="19.5">
+    <row r="256" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A256" s="4" t="s">
         <v>16</v>
       </c>
@@ -5921,7 +5931,7 @@
       <c r="K256" s="10"/>
       <c r="L256" s="10"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="257" customHeight="1" ht="19.5">
+    <row r="257" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A257" s="4" t="s">
         <v>16</v>
       </c>
@@ -5941,7 +5951,7 @@
       <c r="K257" s="10"/>
       <c r="L257" s="10"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="258" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="258" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A258" s="4" t="s">
         <v>16</v>
       </c>
@@ -5961,7 +5971,7 @@
       <c r="K258" s="3"/>
       <c r="L258" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="259" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="259" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A259" s="4" t="s">
         <v>16</v>
       </c>
@@ -5981,7 +5991,7 @@
       <c r="K259" s="3"/>
       <c r="L259" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="260" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="260" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A260" s="4" t="s">
         <v>16</v>
       </c>
@@ -6001,7 +6011,7 @@
       <c r="K260" s="3"/>
       <c r="L260" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="261" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="261" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A261" s="4" t="s">
         <v>16</v>
       </c>
@@ -6021,7 +6031,7 @@
       <c r="K261" s="3"/>
       <c r="L261" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="262" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="262" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A262" s="4" t="s">
         <v>16</v>
       </c>
@@ -6041,7 +6051,7 @@
       <c r="K262" s="3"/>
       <c r="L262" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="263" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="263" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A263" s="4" t="s">
         <v>16</v>
       </c>
@@ -6061,7 +6071,7 @@
       <c r="K263" s="3"/>
       <c r="L263" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="264" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="264" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A264" s="4" t="s">
         <v>16</v>
       </c>
@@ -6081,7 +6091,7 @@
       <c r="K264" s="3"/>
       <c r="L264" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="265" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="265" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A265" s="4" t="s">
         <v>16</v>
       </c>
@@ -6101,7 +6111,7 @@
       <c r="K265" s="3"/>
       <c r="L265" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="266" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="266" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A266" s="4" t="s">
         <v>16</v>
       </c>
@@ -6121,7 +6131,7 @@
       <c r="K266" s="3"/>
       <c r="L266" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="267" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="267" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A267" s="4" t="s">
         <v>16</v>
       </c>
@@ -6141,7 +6151,7 @@
       <c r="K267" s="3"/>
       <c r="L267" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="268" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="268" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A268" s="4" t="s">
         <v>16</v>
       </c>
@@ -6161,7 +6171,7 @@
       <c r="K268" s="3"/>
       <c r="L268" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="269" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="269" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A269" s="4" t="s">
         <v>16</v>
       </c>
@@ -6181,7 +6191,7 @@
       <c r="K269" s="3"/>
       <c r="L269" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="270" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="270" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A270" s="4" t="s">
         <v>16</v>
       </c>
@@ -6201,7 +6211,7 @@
       <c r="K270" s="3"/>
       <c r="L270" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="271" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="271" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A271" s="4" t="s">
         <v>16</v>
       </c>
@@ -6221,7 +6231,7 @@
       <c r="K271" s="3"/>
       <c r="L271" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="272" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="272" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A272" s="4" t="s">
         <v>16</v>
       </c>
@@ -6241,7 +6251,7 @@
       <c r="K272" s="3"/>
       <c r="L272" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="273" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="273" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A273" s="4" t="s">
         <v>16</v>
       </c>
@@ -6261,7 +6271,7 @@
       <c r="K273" s="3"/>
       <c r="L273" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="274" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="274" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A274" s="4" t="s">
         <v>16</v>
       </c>
@@ -6281,7 +6291,7 @@
       <c r="K274" s="3"/>
       <c r="L274" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="275" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="275" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A275" s="4" t="s">
         <v>16</v>
       </c>
@@ -6301,7 +6311,7 @@
       <c r="K275" s="3"/>
       <c r="L275" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="276" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="276" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A276" s="4" t="s">
         <v>16</v>
       </c>
@@ -6321,7 +6331,7 @@
       <c r="K276" s="3"/>
       <c r="L276" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="277" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="277" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A277" s="4" t="s">
         <v>16</v>
       </c>
@@ -6341,7 +6351,7 @@
       <c r="K277" s="3"/>
       <c r="L277" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="278" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="278" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A278" s="4" t="s">
         <v>16</v>
       </c>
@@ -6361,7 +6371,7 @@
       <c r="K278" s="3"/>
       <c r="L278" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="279" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="279" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A279" s="4" t="s">
         <v>16</v>
       </c>
@@ -6381,7 +6391,7 @@
       <c r="K279" s="3"/>
       <c r="L279" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="280" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="280" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A280" s="4" t="s">
         <v>16</v>
       </c>
@@ -6401,7 +6411,7 @@
       <c r="K280" s="3"/>
       <c r="L280" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="281" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="281" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A281" s="4" t="s">
         <v>16</v>
       </c>
@@ -6421,7 +6431,7 @@
       <c r="K281" s="3"/>
       <c r="L281" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="282" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="282" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A282" s="4" t="s">
         <v>16</v>
       </c>
@@ -6441,7 +6451,7 @@
       <c r="K282" s="3"/>
       <c r="L282" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="283" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="283" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A283" s="4" t="s">
         <v>16</v>
       </c>
@@ -6461,7 +6471,7 @@
       <c r="K283" s="3"/>
       <c r="L283" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="284" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="284" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A284" s="4" t="s">
         <v>16</v>
       </c>
@@ -6481,7 +6491,7 @@
       <c r="K284" s="3"/>
       <c r="L284" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="285" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="285" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A285" s="4" t="s">
         <v>16</v>
       </c>
@@ -6501,7 +6511,7 @@
       <c r="K285" s="3"/>
       <c r="L285" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="286" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="286" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A286" s="4" t="s">
         <v>16</v>
       </c>
@@ -6521,7 +6531,7 @@
       <c r="K286" s="3"/>
       <c r="L286" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="287" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="287" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A287" s="4" t="s">
         <v>16</v>
       </c>
@@ -6541,7 +6551,7 @@
       <c r="K287" s="3"/>
       <c r="L287" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="288" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="288" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A288" s="4" t="s">
         <v>16</v>
       </c>
@@ -6561,7 +6571,7 @@
       <c r="K288" s="3"/>
       <c r="L288" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="289" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="289" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A289" s="4" t="s">
         <v>16</v>
       </c>
@@ -6581,7 +6591,7 @@
       <c r="K289" s="3"/>
       <c r="L289" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="290" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="290" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A290" s="4" t="s">
         <v>16</v>
       </c>
@@ -6601,7 +6611,7 @@
       <c r="K290" s="3"/>
       <c r="L290" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="291" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="291" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A291" s="4" t="s">
         <v>16</v>
       </c>
@@ -6621,7 +6631,7 @@
       <c r="K291" s="3"/>
       <c r="L291" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="292" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="292" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A292" s="4" t="s">
         <v>16</v>
       </c>
@@ -6641,7 +6651,7 @@
       <c r="K292" s="3"/>
       <c r="L292" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="293" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row r="293" spans="1:12" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A293" s="4" t="s">
         <v>16</v>
       </c>
@@ -6661,7 +6671,7 @@
       <c r="K293" s="3"/>
       <c r="L293" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="294" customHeight="1" ht="19.5">
+    <row r="294" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A294" s="4"/>
       <c r="B294" s="6"/>
       <c r="C294" s="4" t="s">

</xml_diff>